<commit_message>
add micro-rna doc title
</commit_message>
<xml_diff>
--- a/docs/iplm/docs.xlsx
+++ b/docs/iplm/docs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fourier Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro-rna</t>
   </si>
   <si>
     <t xml:space="preserve">MicroRNAs in Type 1 Diabetes</t>
@@ -217,8 +220,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9:D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -365,8 +368,11 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>

</xml_diff>